<commit_message>
Updates for functionality to work up until PyPSA solves. WIP
</commit_message>
<xml_diff>
--- a/scenarios/ME IRP 2024/scenarios_to_run.xlsx
+++ b/scenarios/ME IRP 2024/scenarios_to_run.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\clhar\showcase\pypsa-rsa\scenarios\ME IRP 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11659C60-9EA8-43AA-B00A-61BF225B4CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602D3CC9-7B6B-4DD1-8AEF-9BB2B6056569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="116">
   <si>
     <t>wildcard</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>none</t>
-  </si>
-  <si>
-    <t>DMD_IRP23</t>
   </si>
   <si>
     <t>RES_MRGN_10</t>
@@ -1067,10 +1064,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DA3024-0964-4665-88DA-35833F91F7A9}">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2:V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,7 +1148,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>17</v>
@@ -1160,10 +1157,10 @@
         <v>18</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>19</v>
@@ -1174,13 +1171,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1192,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>23</v>
@@ -1204,31 +1201,31 @@
         <v>23</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>26</v>
@@ -1237,24 +1234,24 @@
         <v>23</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -1266,7 +1263,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>23</v>
@@ -1278,23 +1275,23 @@
         <v>23</v>
       </c>
       <c r="K3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1302,7 +1299,7 @@
         <v>23</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>26</v>
@@ -1311,24 +1308,24 @@
         <v>23</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -1340,7 +1337,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>23</v>
@@ -1352,22 +1349,22 @@
         <v>23</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>23</v>
@@ -1385,24 +1382,24 @@
         <v>23</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X4" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1414,7 +1411,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>23</v>
@@ -1426,28 +1423,28 @@
         <v>23</v>
       </c>
       <c r="K5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="R5" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S5" s="10" t="s">
         <v>23</v>
@@ -1459,24 +1456,24 @@
         <v>23</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X5" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -1488,7 +1485,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>23</v>
@@ -1500,28 +1497,28 @@
         <v>23</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q6" s="7" t="s">
         <v>23</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S6" s="10" t="s">
         <v>23</v>
@@ -1533,24 +1530,24 @@
         <v>23</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X6" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X6" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -1562,7 +1559,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>23</v>
@@ -1574,28 +1571,28 @@
         <v>23</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S7" s="10" t="s">
         <v>23</v>
@@ -1607,24 +1604,24 @@
         <v>23</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X7" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1636,7 +1633,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>23</v>
@@ -1648,28 +1645,28 @@
         <v>23</v>
       </c>
       <c r="K8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="M8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S8" s="10" t="s">
         <v>23</v>
@@ -1681,24 +1678,24 @@
         <v>23</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1710,7 +1707,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>23</v>
@@ -1722,23 +1719,23 @@
         <v>23</v>
       </c>
       <c r="K9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="M9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>23</v>
       </c>
       <c r="S9" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T9" s="7" t="s">
         <v>26</v>
@@ -1755,24 +1752,24 @@
         <v>23</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1784,7 +1781,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>23</v>
@@ -1796,13 +1793,13 @@
         <v>23</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>24</v>
@@ -1811,7 +1808,7 @@
         <v>24</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="7" t="s">
         <v>23</v>
@@ -1820,7 +1817,7 @@
         <v>23</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>26</v>
@@ -1829,24 +1826,24 @@
         <v>23</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X10" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X10" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -1858,7 +1855,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>23</v>
@@ -1870,13 +1867,13 @@
         <v>23</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>24</v>
@@ -1885,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q11" s="7" t="s">
         <v>23</v>
@@ -1894,7 +1891,7 @@
         <v>23</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T11" s="7" t="s">
         <v>26</v>
@@ -1903,24 +1900,24 @@
         <v>23</v>
       </c>
       <c r="V11" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W11" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X11" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -1932,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>23</v>
@@ -1944,23 +1941,23 @@
         <v>23</v>
       </c>
       <c r="K12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1968,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T12" s="7" t="s">
         <v>26</v>
@@ -1977,24 +1974,24 @@
         <v>23</v>
       </c>
       <c r="V12" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W12" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X12" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -2006,7 +2003,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>23</v>
@@ -2018,22 +2015,22 @@
         <v>23</v>
       </c>
       <c r="K13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="12" t="s">
+      <c r="N13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="Q13" s="7" t="s">
         <v>23</v>
@@ -2051,24 +2048,24 @@
         <v>23</v>
       </c>
       <c r="V13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W13" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X13" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -2080,7 +2077,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>23</v>
@@ -2092,13 +2089,13 @@
         <v>23</v>
       </c>
       <c r="K14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="N14" s="7" t="str">
         <f>N13</f>
@@ -2108,7 +2105,7 @@
         <v>24</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q14" s="7" t="s">
         <v>23</v>
@@ -2117,7 +2114,7 @@
         <v>23</v>
       </c>
       <c r="S14" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T14" s="7" t="s">
         <v>26</v>
@@ -2126,24 +2123,24 @@
         <v>23</v>
       </c>
       <c r="V14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W14" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -2155,7 +2152,7 @@
         <v>22</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>23</v>
@@ -2167,23 +2164,23 @@
         <v>23</v>
       </c>
       <c r="K15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M15" s="12" t="s">
+      <c r="N15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="N15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q15" s="7" t="s">
         <v>23</v>
       </c>
@@ -2191,7 +2188,7 @@
         <v>23</v>
       </c>
       <c r="S15" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>26</v>
@@ -2200,24 +2197,24 @@
         <v>23</v>
       </c>
       <c r="V15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W15" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X15" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -2229,7 +2226,7 @@
         <v>22</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>23</v>
@@ -2241,22 +2238,22 @@
         <v>23</v>
       </c>
       <c r="K16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="12" t="s">
+      <c r="N16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>23</v>
@@ -2274,24 +2271,24 @@
         <v>23</v>
       </c>
       <c r="V16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X16" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -2303,43 +2300,43 @@
         <v>22</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="M17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="Q17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S17" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>26</v>
@@ -2348,24 +2345,24 @@
         <v>23</v>
       </c>
       <c r="V17" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X17" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X17" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -2377,25 +2374,25 @@
         <v>22</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>24</v>
@@ -2404,7 +2401,7 @@
         <v>24</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q18" s="7" t="s">
         <v>23</v>
@@ -2413,7 +2410,7 @@
         <v>23</v>
       </c>
       <c r="S18" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T18" s="7" t="s">
         <v>26</v>
@@ -2422,24 +2419,24 @@
         <v>23</v>
       </c>
       <c r="V18" s="12" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="W18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X18" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X18" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -2451,25 +2448,25 @@
         <v>22</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>24</v>
@@ -2478,7 +2475,7 @@
         <v>24</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q19" s="7" t="s">
         <v>23</v>
@@ -2487,7 +2484,7 @@
         <v>23</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>26</v>
@@ -2496,24 +2493,24 @@
         <v>23</v>
       </c>
       <c r="V19" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W19" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="X19" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
@@ -2525,35 +2522,35 @@
         <v>22</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M20" s="12" t="s">
+      <c r="N20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="N20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q20" s="7" t="s">
         <v>23</v>
       </c>
@@ -2561,7 +2558,7 @@
         <v>23</v>
       </c>
       <c r="S20" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T20" s="7" t="s">
         <v>26</v>
@@ -2570,24 +2567,24 @@
         <v>23</v>
       </c>
       <c r="V20" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W20" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X20" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -2599,34 +2596,34 @@
         <v>22</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="12" t="s">
+      <c r="N21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P21" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="Q21" s="7" t="s">
         <v>23</v>
@@ -2644,24 +2641,24 @@
         <v>23</v>
       </c>
       <c r="V21" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W21" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X21" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
@@ -2673,25 +2670,25 @@
         <v>22</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M22" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="N22" s="7" t="str">
         <f>N21</f>
@@ -2701,7 +2698,7 @@
         <v>24</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q22" s="7" t="s">
         <v>23</v>
@@ -2710,7 +2707,7 @@
         <v>23</v>
       </c>
       <c r="S22" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>26</v>
@@ -2719,24 +2716,24 @@
         <v>23</v>
       </c>
       <c r="V22" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W22" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X22" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -2748,34 +2745,34 @@
         <v>22</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L23" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="12" t="s">
+      <c r="N23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P23" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P23" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>23</v>
@@ -2793,24 +2790,24 @@
         <v>23</v>
       </c>
       <c r="V23" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W23" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X23" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -2822,7 +2819,7 @@
         <v>22</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>23</v>
@@ -2834,31 +2831,31 @@
         <v>23</v>
       </c>
       <c r="K24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N24" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P24" s="28" t="s">
+      <c r="Q24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="T24" s="7" t="s">
         <v>26</v>
@@ -2867,24 +2864,24 @@
         <v>23</v>
       </c>
       <c r="V24" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W24" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X24" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
@@ -2896,7 +2893,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>23</v>
@@ -2908,7 +2905,7 @@
         <v>23</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L25" s="18" t="s">
         <v>24</v>
@@ -2932,7 +2929,7 @@
         <v>23</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>26</v>
@@ -2941,7 +2938,7 @@
         <v>23</v>
       </c>
       <c r="V25" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W25" s="13" t="str">
         <f t="shared" ref="W25:X29" si="0">W24</f>
@@ -2954,13 +2951,13 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
@@ -2972,7 +2969,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>23</v>
@@ -2984,16 +2981,16 @@
         <v>23</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L26" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N26" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>24</v>
@@ -3017,7 +3014,7 @@
         <v>23</v>
       </c>
       <c r="V26" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W26" s="13" t="str">
         <f t="shared" si="0"/>
@@ -3030,13 +3027,13 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
@@ -3048,7 +3045,7 @@
         <v>22</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>23</v>
@@ -3060,16 +3057,16 @@
         <v>23</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O27" s="7" t="s">
         <v>24</v>
@@ -3093,7 +3090,7 @@
         <v>23</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W27" s="13" t="str">
         <f t="shared" si="0"/>
@@ -3106,13 +3103,13 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
@@ -3124,7 +3121,7 @@
         <v>22</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>23</v>
@@ -3136,16 +3133,16 @@
         <v>23</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L28" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>24</v>
@@ -3169,7 +3166,7 @@
         <v>23</v>
       </c>
       <c r="V28" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W28" s="13" t="str">
         <f t="shared" si="0"/>
@@ -3182,13 +3179,13 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="6">
         <v>1</v>
@@ -3200,7 +3197,7 @@
         <v>22</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>23</v>
@@ -3212,16 +3209,16 @@
         <v>23</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L29" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N29" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O29" s="7" t="s">
         <v>24</v>
@@ -3245,7 +3242,7 @@
         <v>23</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W29" s="13" t="str">
         <f t="shared" si="0"/>
@@ -3258,13 +3255,13 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
@@ -3276,7 +3273,7 @@
         <v>22</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>23</v>
@@ -3288,16 +3285,16 @@
         <v>23</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L30" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O30" s="7" t="s">
         <v>24</v>
@@ -3312,7 +3309,7 @@
         <v>23</v>
       </c>
       <c r="S30" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T30" s="7" t="s">
         <v>26</v>
@@ -3321,7 +3318,7 @@
         <v>23</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W30" s="13" t="str">
         <f>W28</f>
@@ -3334,13 +3331,13 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="6">
         <v>1</v>
@@ -3352,7 +3349,7 @@
         <v>22</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>23</v>
@@ -3364,16 +3361,16 @@
         <v>23</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L31" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O31" s="7" t="s">
         <v>24</v>
@@ -3388,7 +3385,7 @@
         <v>23</v>
       </c>
       <c r="S31" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T31" s="7" t="s">
         <v>26</v>
@@ -3397,7 +3394,7 @@
         <v>23</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W31" s="13" t="str">
         <f>W30</f>
@@ -3410,13 +3407,13 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="6">
         <v>1</v>
@@ -3428,7 +3425,7 @@
         <v>22</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>23</v>
@@ -3440,16 +3437,16 @@
         <v>23</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L32" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O32" s="7" t="s">
         <v>24</v>
@@ -3464,7 +3461,7 @@
         <v>23</v>
       </c>
       <c r="S32" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T32" s="7" t="s">
         <v>26</v>
@@ -3473,7 +3470,7 @@
         <v>23</v>
       </c>
       <c r="V32" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W32" s="13" t="str">
         <f>W30</f>
@@ -3486,13 +3483,13 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="6">
         <v>1</v>
@@ -3504,7 +3501,7 @@
         <v>22</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>23</v>
@@ -3516,16 +3513,16 @@
         <v>23</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L33" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>24</v>
@@ -3537,7 +3534,7 @@
         <v>23</v>
       </c>
       <c r="R33" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S33" s="10" t="s">
         <v>23</v>
@@ -3549,7 +3546,7 @@
         <v>23</v>
       </c>
       <c r="V33" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W33" s="13" t="str">
         <f>W32</f>
@@ -3562,7 +3559,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" s="16" t="b">
         <v>0</v>
@@ -3581,7 +3578,7 @@
         <v>22</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>23</v>
@@ -3593,16 +3590,16 @@
         <v>23</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O34" s="7" t="s">
         <v>24</v>
@@ -3614,7 +3611,7 @@
         <v>23</v>
       </c>
       <c r="R34" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S34" s="10" t="s">
         <v>23</v>
@@ -3626,7 +3623,7 @@
         <v>23</v>
       </c>
       <c r="V34" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W34" s="13" t="str">
         <f>W33</f>
@@ -3639,7 +3636,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="16" t="b">
         <v>0</v>
@@ -3658,7 +3655,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>23</v>
@@ -3670,16 +3667,16 @@
         <v>23</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O35" s="7" t="s">
         <v>24</v>
@@ -3691,7 +3688,7 @@
         <v>23</v>
       </c>
       <c r="R35" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S35" s="10" t="s">
         <v>23</v>
@@ -3703,7 +3700,7 @@
         <v>23</v>
       </c>
       <c r="V35" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W35" s="13" t="str">
         <f>W34</f>
@@ -3716,7 +3713,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="16" t="b">
         <v>0</v>
@@ -3735,7 +3732,7 @@
         <v>22</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>23</v>
@@ -3747,16 +3744,16 @@
         <v>23</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M36" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O36" s="7" t="s">
         <v>24</v>
@@ -3768,7 +3765,7 @@
         <v>23</v>
       </c>
       <c r="R36" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S36" s="10" t="s">
         <v>23</v>
@@ -3780,7 +3777,7 @@
         <v>23</v>
       </c>
       <c r="V36" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W36" s="13" t="str">
         <f>W35</f>
@@ -3793,13 +3790,13 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="6">
         <v>1</v>
@@ -3811,10 +3808,10 @@
         <v>22</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>23</v>
@@ -3823,16 +3820,16 @@
         <v>23</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N37" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O37" s="7" t="s">
         <v>24</v>
@@ -3850,13 +3847,13 @@
         <v>23</v>
       </c>
       <c r="T37" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U37" s="11" t="s">
         <v>23</v>
       </c>
       <c r="V37" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W37" s="13" t="str">
         <f>W35</f>
@@ -3869,7 +3866,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="16" t="b">
         <v>0</v>
@@ -3888,10 +3885,10 @@
         <v>22</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>23</v>
@@ -3900,16 +3897,16 @@
         <v>23</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M38" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N38" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O38" s="7" t="s">
         <v>24</v>
@@ -3927,13 +3924,13 @@
         <v>23</v>
       </c>
       <c r="T38" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U38" s="11" t="s">
         <v>23</v>
       </c>
       <c r="V38" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W38" s="13" t="str">
         <f>W37</f>
@@ -3946,13 +3943,13 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -3964,10 +3961,10 @@
         <v>22</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>23</v>
@@ -3976,16 +3973,16 @@
         <v>23</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M39" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N39" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O39" s="7" t="s">
         <v>24</v>
@@ -4000,7 +3997,7 @@
         <v>23</v>
       </c>
       <c r="S39" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T39" s="7" t="s">
         <v>26</v>
@@ -4009,7 +4006,7 @@
         <v>23</v>
       </c>
       <c r="V39" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W39" s="13" t="str">
         <f>W36</f>
@@ -4022,13 +4019,13 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="6">
         <v>1</v>
@@ -4040,10 +4037,10 @@
         <v>22</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>23</v>
@@ -4052,16 +4049,16 @@
         <v>23</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L40" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M40" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N40" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O40" s="7" t="s">
         <v>24</v>
@@ -4079,13 +4076,13 @@
         <v>23</v>
       </c>
       <c r="T40" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U40" s="11" t="s">
         <v>23</v>
       </c>
       <c r="V40" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W40" s="13" t="str">
         <f>W38</f>
@@ -4098,13 +4095,13 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="6">
         <v>1</v>
@@ -4116,10 +4113,10 @@
         <v>22</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>23</v>
@@ -4128,16 +4125,16 @@
         <v>23</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L41" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N41" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O41" s="7" t="s">
         <v>24</v>
@@ -4155,13 +4152,13 @@
         <v>23</v>
       </c>
       <c r="T41" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U41" s="11" t="s">
         <v>23</v>
       </c>
       <c r="V41" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W41" s="13" t="str">
         <f>W40</f>
@@ -4174,13 +4171,13 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="6">
         <v>1</v>
@@ -4192,10 +4189,10 @@
         <v>22</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>23</v>
@@ -4204,16 +4201,16 @@
         <v>23</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M42" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N42" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O42" s="7" t="s">
         <v>24</v>
@@ -4237,7 +4234,7 @@
         <v>23</v>
       </c>
       <c r="V42" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W42" s="13" t="str">
         <f>W39</f>
@@ -4250,13 +4247,13 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="6">
         <v>1</v>
@@ -4268,10 +4265,10 @@
         <v>22</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>23</v>
@@ -4280,16 +4277,16 @@
         <v>23</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M43" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N43" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O43" s="7" t="s">
         <v>24</v>
@@ -4304,7 +4301,7 @@
         <v>23</v>
       </c>
       <c r="S43" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>26</v>
@@ -4313,7 +4310,7 @@
         <v>23</v>
       </c>
       <c r="V43" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W43" s="13" t="str">
         <f>W40</f>
@@ -4326,13 +4323,13 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="6">
         <v>1</v>
@@ -4344,7 +4341,7 @@
         <v>22</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>23</v>
@@ -4356,16 +4353,16 @@
         <v>23</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M44" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N44" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O44" s="7" t="s">
         <v>24</v>
@@ -4380,7 +4377,7 @@
         <v>23</v>
       </c>
       <c r="S44" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T44" s="7" t="s">
         <v>26</v>
@@ -4389,7 +4386,7 @@
         <v>23</v>
       </c>
       <c r="V44" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W44" s="13" t="str">
         <f>W41</f>
@@ -4402,13 +4399,13 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="6">
         <v>1</v>
@@ -4420,7 +4417,7 @@
         <v>22</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>23</v>
@@ -4432,23 +4429,23 @@
         <v>23</v>
       </c>
       <c r="K45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="M45" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P45" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M45" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N45" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O45" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P45" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="Q45" s="7" t="s">
         <v>23</v>
       </c>
@@ -4456,7 +4453,7 @@
         <v>23</v>
       </c>
       <c r="S45" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T45" s="7" t="s">
         <v>26</v>
@@ -4465,24 +4462,24 @@
         <v>23</v>
       </c>
       <c r="V45" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W45" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X45" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X45" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="6">
         <v>1</v>
@@ -4494,10 +4491,10 @@
         <v>22</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>23</v>
@@ -4506,16 +4503,16 @@
         <v>23</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L46" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N46" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O46" s="7" t="s">
         <v>24</v>
@@ -4530,7 +4527,7 @@
         <v>23</v>
       </c>
       <c r="S46" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>26</v>
@@ -4539,7 +4536,7 @@
         <v>23</v>
       </c>
       <c r="V46" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W46" s="13" t="str">
         <f>W43</f>
@@ -4552,13 +4549,13 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="6">
         <v>1</v>
@@ -4570,7 +4567,7 @@
         <v>22</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>23</v>
@@ -4582,16 +4579,16 @@
         <v>23</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L47" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N47" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O47" s="7" t="s">
         <v>24</v>
@@ -4606,7 +4603,7 @@
         <v>23</v>
       </c>
       <c r="S47" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T47" s="7" t="s">
         <v>26</v>
@@ -4615,10 +4612,10 @@
         <v>23</v>
       </c>
       <c r="V47" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W47" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X47" s="14" t="str">
         <f>X45</f>
@@ -4627,13 +4624,13 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B48" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="6">
         <v>1</v>
@@ -4645,7 +4642,7 @@
         <v>22</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>23</v>
@@ -4657,13 +4654,13 @@
         <v>23</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N48" s="7" t="s">
         <v>24</v>
@@ -4672,7 +4669,7 @@
         <v>24</v>
       </c>
       <c r="P48" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q48" s="7" t="s">
         <v>23</v>
@@ -4690,24 +4687,24 @@
         <v>23</v>
       </c>
       <c r="V48" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W48" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X48" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="X48" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" s="16" t="b">
         <v>0</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" s="6">
         <v>1</v>
@@ -4719,7 +4716,7 @@
         <v>22</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>23</v>
@@ -4731,16 +4728,16 @@
         <v>23</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L49" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M49" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N49" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O49" s="7" t="s">
         <v>24</v>
@@ -4764,13 +4761,13 @@
         <v>23</v>
       </c>
       <c r="V49" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W49" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X49" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed multi generator definition up until RE generator profiles are added. Also fixed add_electricity mock snakemake for debug purposes
</commit_message>
<xml_diff>
--- a/scenarios/ME IRP 2024/scenarios_to_run.xlsx
+++ b/scenarios/ME IRP 2024/scenarios_to_run.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\clhar\showcase\pypsa-rsa\scenarios\ME IRP 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602D3CC9-7B6B-4DD1-8AEF-9BB2B6056569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670124DC-0FA0-44E4-9720-8C682DE7026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="117">
   <si>
     <t>wildcard</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>IRP2023</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +567,12 @@
         <bgColor rgb="FFB4E5A2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -630,7 +639,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -737,6 +746,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1062,12 +1077,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DA3024-0964-4665-88DA-35833F91F7A9}">
-  <dimension ref="A1:X49"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2:V49"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,10 +1189,11 @@
         <v>33</v>
       </c>
       <c r="B2" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="str">
+        <f>"2025,2030"</f>
+        <v>2025,2030</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -4770,8 +4786,83 @@
         <v>39</v>
       </c>
     </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A50" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="37" t="str">
+        <f>"2025, 2026"</f>
+        <v>2025, 2026</v>
+      </c>
+      <c r="D50" s="6">
+        <v>10</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N50" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P50" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S50" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U50" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="V50" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="W50" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="X50" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B49">
+  <conditionalFormatting sqref="B2:B50">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>